<commit_message>
detecta Arritmias con parametros normales
</commit_message>
<xml_diff>
--- a/DeteccionArritmiasTotal.xlsx
+++ b/DeteccionArritmiasTotal.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6D99B9-5FAE-4BED-9413-DE9060B53A0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F984D3-5AC7-454F-BC19-48CDD63E0106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{D607851B-EE39-4F9F-BF50-C83A55A4E572}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$J$96</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -247,12 +250,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -267,8 +276,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD434795-2931-472D-8A99-953EFB51E76D}">
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="J88" sqref="A88:J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,34 +634,34 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1">
         <v>95.336600000000004</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>100</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>2273</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>2167</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
         <v>106</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>106</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>4.6634000000000002</v>
       </c>
     </row>
@@ -752,34 +762,34 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
         <v>97.942599999999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>100</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>2090</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>2047</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
         <v>43</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>43</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="1">
         <v>2.0573999999999999</v>
       </c>
     </row>
@@ -1104,66 +1114,66 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1">
         <v>95.998400000000004</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>100</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>2549</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="1">
         <v>2447</v>
       </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
         <v>102</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="1">
         <v>102</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
         <v>4.0015999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1">
         <v>95.654600000000002</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>100</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>1795</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="1">
         <v>1717</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
         <v>78</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="1">
         <v>78</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="1">
         <v>4.3453999999999997</v>
       </c>
     </row>
@@ -3376,34 +3386,34 @@
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B88" t="s">
-        <v>11</v>
-      </c>
-      <c r="C88">
+      <c r="B88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" s="1">
         <v>96.833799999999997</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="1">
         <v>66.245500000000007</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="1">
         <v>758</v>
       </c>
-      <c r="F88">
+      <c r="F88" s="1">
         <v>734</v>
       </c>
-      <c r="G88">
+      <c r="G88" s="1">
         <v>374</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="1">
         <v>24</v>
       </c>
-      <c r="I88">
+      <c r="I88" s="1">
         <v>398</v>
       </c>
-      <c r="J88">
+      <c r="J88" s="1">
         <v>52.506599999999999</v>
       </c>
     </row>
@@ -3669,6 +3679,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J96" xr:uid="{5C402FB0-9D75-47A2-B46C-DC817BE3EB6E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pan tompkins, elgendi y boonperm
</commit_message>
<xml_diff>
--- a/DeteccionArritmiasTotal.xlsx
+++ b/DeteccionArritmiasTotal.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Documents\Arritmias\algoritmoArritmias-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D339B964-2F81-4A3A-9209-E1FFEB258134}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01323DF6-6C85-40E1-9DA5-F42C41902E8D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14535" yWindow="345" windowWidth="2400" windowHeight="585" xr2:uid="{4C325BAF-2CF2-414D-8FF5-F6E93F90FF78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{4C325BAF-2CF2-414D-8FF5-F6E93F90FF78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$J$191</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="65">
   <si>
     <t>Registro</t>
   </si>
@@ -235,7 +240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,13 +248,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292E"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -264,8 +287,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +609,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C6E7827-8239-4A26-93D7-F1ED8029C7A1}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="A190" sqref="A190:J191"/>
+    <sheetView topLeftCell="A125" workbookViewId="0">
+      <selection sqref="A1:J190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,7 +746,7 @@
         <v>108.8235</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -812,7 +842,7 @@
         <v>113.8408</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -908,7 +938,7 @@
         <v>50.101100000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -940,7 +970,7 @@
         <v>266.66669999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -972,7 +1002,7 @@
         <v>103.8817</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1196,7 +1226,7 @@
         <v>84.134600000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1388,7 +1418,7 @@
         <v>41.121499999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1548,7 +1578,7 @@
         <v>88.787499999999994</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1612,7 +1642,7 @@
         <v>74.248900000000006</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1644,7 +1674,7 @@
         <v>1673.913</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1708,7 +1738,7 @@
         <v>117.852</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1740,7 +1770,7 @@
         <v>108.0132</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1804,7 +1834,7 @@
         <v>94.322299999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -1836,7 +1866,7 @@
         <v>172.11539999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1868,7 +1898,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -1900,7 +1930,7 @@
         <v>116.2313</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1932,7 +1962,7 @@
         <v>91.964299999999994</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1964,7 +1994,7 @@
         <v>955.69619999999998</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -2028,7 +2058,7 @@
         <v>4.0275999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -2092,7 +2122,7 @@
         <v>99.798000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -2124,7 +2154,7 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -2156,7 +2186,7 @@
         <v>95.762699999999995</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -2220,7 +2250,7 @@
         <v>95.169899999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -2284,7 +2314,7 @@
         <v>49.817799999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -2316,7 +2346,7 @@
         <v>99.233699999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -2348,7 +2378,7 @@
         <v>93.168700000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -2380,7 +2410,7 @@
         <v>10550</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>47</v>
       </c>
@@ -2476,7 +2506,7 @@
         <v>99.585300000000004</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>49</v>
       </c>
@@ -2508,7 +2538,7 @@
         <v>5185.7142999999996</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>49</v>
       </c>
@@ -2572,7 +2602,7 @@
         <v>81.7804</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>50</v>
       </c>
@@ -2604,7 +2634,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>50</v>
       </c>
@@ -2668,7 +2698,7 @@
         <v>99.523399999999995</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>51</v>
       </c>
@@ -2700,7 +2730,7 @@
         <v>16683.333299999998</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>52</v>
       </c>
@@ -2732,7 +2762,7 @@
         <v>100.5917</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>52</v>
       </c>
@@ -2764,7 +2794,7 @@
         <v>10566.6667</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>52</v>
       </c>
@@ -2828,7 +2858,7 @@
         <v>260.7903</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>53</v>
       </c>
@@ -2860,7 +2890,7 @@
         <v>92.7303</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>53</v>
       </c>
@@ -2924,7 +2954,7 @@
         <v>66.749099999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>54</v>
       </c>
@@ -2956,7 +2986,7 @@
         <v>3244.4443999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -2988,7 +3018,7 @@
         <v>87.993200000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>55</v>
       </c>
@@ -3020,7 +3050,7 @@
         <v>10583.3333</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>55</v>
       </c>
@@ -3084,7 +3114,7 @@
         <v>37.341200000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>56</v>
       </c>
@@ -3116,7 +3146,7 @@
         <v>92.183300000000003</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>56</v>
       </c>
@@ -3148,7 +3178,7 @@
         <v>351.06380000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>56</v>
       </c>
@@ -3212,7 +3242,7 @@
         <v>58.1663</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>57</v>
       </c>
@@ -3244,7 +3274,7 @@
         <v>497.23759999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>57</v>
       </c>
@@ -3308,7 +3338,7 @@
         <v>89.692599999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>58</v>
       </c>
@@ -3372,7 +3402,7 @@
         <v>42.953000000000003</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>59</v>
       </c>
@@ -3436,7 +3466,7 @@
         <v>9.2094000000000005</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>60</v>
       </c>
@@ -3468,7 +3498,7 @@
         <v>103.09520000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>61</v>
       </c>
@@ -3532,7 +3562,7 @@
         <v>94.113500000000002</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>63</v>
       </c>
@@ -3564,7 +3594,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>63</v>
       </c>
@@ -3628,7 +3658,7 @@
         <v>4.4024999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>64</v>
       </c>
@@ -3756,7 +3786,7 @@
         <v>108.8235</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>13</v>
       </c>
@@ -3852,7 +3882,7 @@
         <v>113.8408</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>16</v>
       </c>
@@ -3948,7 +3978,7 @@
         <v>50.101100000000002</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>18</v>
       </c>
@@ -3980,7 +4010,7 @@
         <v>266.66669999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>18</v>
       </c>
@@ -4012,7 +4042,7 @@
         <v>103.8817</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>20</v>
       </c>
@@ -4236,7 +4266,7 @@
         <v>84.134600000000006</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>26</v>
       </c>
@@ -4428,7 +4458,7 @@
         <v>41.121499999999997</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>31</v>
       </c>
@@ -4588,7 +4618,7 @@
         <v>88.787499999999994</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>35</v>
       </c>
@@ -4652,7 +4682,7 @@
         <v>74.248900000000006</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>36</v>
       </c>
@@ -4684,7 +4714,7 @@
         <v>1673.913</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>36</v>
       </c>
@@ -4748,7 +4778,7 @@
         <v>117.852</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>37</v>
       </c>
@@ -4780,7 +4810,7 @@
         <v>108.0132</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>37</v>
       </c>
@@ -4844,7 +4874,7 @@
         <v>94.322299999999998</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>39</v>
       </c>
@@ -4876,7 +4906,7 @@
         <v>172.11539999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>39</v>
       </c>
@@ -4908,7 +4938,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>41</v>
       </c>
@@ -4940,7 +4970,7 @@
         <v>116.2313</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>41</v>
       </c>
@@ -4972,7 +5002,7 @@
         <v>91.964299999999994</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>41</v>
       </c>
@@ -5004,7 +5034,7 @@
         <v>955.69619999999998</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>41</v>
       </c>
@@ -5068,7 +5098,7 @@
         <v>4.0275999999999996</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>42</v>
       </c>
@@ -5132,7 +5162,7 @@
         <v>99.798000000000002</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>43</v>
       </c>
@@ -5164,7 +5194,7 @@
         <v>8300</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>43</v>
       </c>
@@ -5196,7 +5226,7 @@
         <v>95.762699999999995</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>43</v>
       </c>
@@ -5260,7 +5290,7 @@
         <v>95.169899999999998</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>45</v>
       </c>
@@ -5324,7 +5354,7 @@
         <v>49.817799999999998</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>46</v>
       </c>
@@ -5356,7 +5386,7 @@
         <v>99.233699999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>47</v>
       </c>
@@ -5388,7 +5418,7 @@
         <v>93.168700000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>47</v>
       </c>
@@ -5420,7 +5450,7 @@
         <v>10550</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>47</v>
       </c>
@@ -5516,7 +5546,7 @@
         <v>99.585300000000004</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>49</v>
       </c>
@@ -5548,7 +5578,7 @@
         <v>5185.7142999999996</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>49</v>
       </c>
@@ -5612,7 +5642,7 @@
         <v>81.7804</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>50</v>
       </c>
@@ -5644,7 +5674,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>50</v>
       </c>
@@ -5708,7 +5738,7 @@
         <v>99.523399999999995</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>51</v>
       </c>
@@ -5740,7 +5770,7 @@
         <v>16683.333299999998</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>52</v>
       </c>
@@ -5772,7 +5802,7 @@
         <v>100.5917</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>52</v>
       </c>
@@ -5804,7 +5834,7 @@
         <v>10566.6667</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>52</v>
       </c>
@@ -5868,7 +5898,7 @@
         <v>260.7903</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>53</v>
       </c>
@@ -5900,7 +5930,7 @@
         <v>92.7303</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>53</v>
       </c>
@@ -5964,7 +5994,7 @@
         <v>66.749099999999999</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>54</v>
       </c>
@@ -5996,7 +6026,7 @@
         <v>3244.4443999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>55</v>
       </c>
@@ -6028,7 +6058,7 @@
         <v>87.993200000000002</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>55</v>
       </c>
@@ -6060,7 +6090,7 @@
         <v>10583.3333</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>55</v>
       </c>
@@ -6124,7 +6154,7 @@
         <v>37.341200000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>56</v>
       </c>
@@ -6156,7 +6186,7 @@
         <v>92.183300000000003</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>56</v>
       </c>
@@ -6188,7 +6218,7 @@
         <v>351.06380000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>56</v>
       </c>
@@ -6252,7 +6282,7 @@
         <v>58.1663</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>57</v>
       </c>
@@ -6284,7 +6314,7 @@
         <v>497.23759999999999</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>57</v>
       </c>
@@ -6348,7 +6378,7 @@
         <v>89.692599999999999</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>58</v>
       </c>
@@ -6412,7 +6442,7 @@
         <v>42.953000000000003</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>59</v>
       </c>
@@ -6476,7 +6506,7 @@
         <v>9.2094000000000005</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>60</v>
       </c>
@@ -6508,7 +6538,7 @@
         <v>103.09520000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>61</v>
       </c>
@@ -6572,7 +6602,7 @@
         <v>94.113500000000002</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>63</v>
       </c>
@@ -6604,7 +6634,7 @@
         <v>4500</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>63</v>
       </c>
@@ -6668,7 +6698,7 @@
         <v>4.4024999999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>64</v>
       </c>
@@ -6698,6 +6728,2931 @@
       </c>
       <c r="J191">
         <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:J191" xr:uid="{795BCC06-70E3-4BAD-9944-60ECEE581F67}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Ritmo Sinusal Normal"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2DA5D21-2274-47C4-864B-28980C75358D}">
+  <dimension ref="A1:S50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+    </row>
+    <row r="2" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2187</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>54.676299999999998</v>
+      </c>
+      <c r="E2">
+        <v>95.878900000000002</v>
+      </c>
+      <c r="F2">
+        <v>2085</v>
+      </c>
+      <c r="G2">
+        <v>1140</v>
+      </c>
+      <c r="H2">
+        <v>49</v>
+      </c>
+      <c r="I2">
+        <v>945</v>
+      </c>
+      <c r="J2">
+        <v>994</v>
+      </c>
+      <c r="K2">
+        <v>47.673900000000003</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2229</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>33.762900000000002</v>
+      </c>
+      <c r="E3">
+        <v>81.875</v>
+      </c>
+      <c r="F3">
+        <v>1940</v>
+      </c>
+      <c r="G3">
+        <v>655</v>
+      </c>
+      <c r="H3">
+        <v>145</v>
+      </c>
+      <c r="I3">
+        <v>1285</v>
+      </c>
+      <c r="J3">
+        <v>1430</v>
+      </c>
+      <c r="K3">
+        <v>73.711299999999994</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2027</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>54.898299999999999</v>
+      </c>
+      <c r="E4">
+        <v>48.292700000000004</v>
+      </c>
+      <c r="F4">
+        <v>541</v>
+      </c>
+      <c r="G4">
+        <v>297</v>
+      </c>
+      <c r="H4">
+        <v>318</v>
+      </c>
+      <c r="I4">
+        <v>244</v>
+      </c>
+      <c r="J4">
+        <v>562</v>
+      </c>
+      <c r="K4">
+        <v>103.8817</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2137</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>95.5077</v>
+      </c>
+      <c r="E5">
+        <v>99.804400000000001</v>
+      </c>
+      <c r="F5">
+        <v>2137</v>
+      </c>
+      <c r="G5">
+        <v>2041</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>96</v>
+      </c>
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="K5">
+        <v>4.6795</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1879</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>57.142899999999997</v>
+      </c>
+      <c r="E6">
+        <v>0.27951999999999999</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>1427</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>1430</v>
+      </c>
+      <c r="K6">
+        <v>20428.571400000001</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1987</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>42.535800000000002</v>
+      </c>
+      <c r="E7">
+        <v>50.6083</v>
+      </c>
+      <c r="F7">
+        <v>489</v>
+      </c>
+      <c r="G7">
+        <v>208</v>
+      </c>
+      <c r="H7">
+        <v>203</v>
+      </c>
+      <c r="I7">
+        <v>281</v>
+      </c>
+      <c r="J7">
+        <v>484</v>
+      </c>
+      <c r="K7">
+        <v>98.977500000000006</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1619</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>61.176499999999997</v>
+      </c>
+      <c r="E8">
+        <v>8.7394999999999996</v>
+      </c>
+      <c r="F8">
+        <v>85</v>
+      </c>
+      <c r="G8">
+        <v>52</v>
+      </c>
+      <c r="H8">
+        <v>543</v>
+      </c>
+      <c r="I8">
+        <v>33</v>
+      </c>
+      <c r="J8">
+        <v>576</v>
+      </c>
+      <c r="K8">
+        <v>677.64710000000002</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2601</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>29.830500000000001</v>
+      </c>
+      <c r="E9">
+        <v>75.536500000000004</v>
+      </c>
+      <c r="F9">
+        <v>1180</v>
+      </c>
+      <c r="G9">
+        <v>352</v>
+      </c>
+      <c r="H9">
+        <v>114</v>
+      </c>
+      <c r="I9">
+        <v>828</v>
+      </c>
+      <c r="J9">
+        <v>942</v>
+      </c>
+      <c r="K9">
+        <v>79.830500000000001</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1961</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>50.969499999999996</v>
+      </c>
+      <c r="E10">
+        <v>28.264199999999999</v>
+      </c>
+      <c r="F10">
+        <v>361</v>
+      </c>
+      <c r="G10">
+        <v>184</v>
+      </c>
+      <c r="H10">
+        <v>467</v>
+      </c>
+      <c r="I10">
+        <v>177</v>
+      </c>
+      <c r="J10">
+        <v>644</v>
+      </c>
+      <c r="K10">
+        <v>178.39340000000001</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2974</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>14.2857</v>
+      </c>
+      <c r="E11">
+        <v>0.12755</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>783</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>789</v>
+      </c>
+      <c r="K11">
+        <v>11271.428599999999</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2332</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>41.192399999999999</v>
+      </c>
+      <c r="E12">
+        <v>10.7042</v>
+      </c>
+      <c r="F12">
+        <v>369</v>
+      </c>
+      <c r="G12">
+        <v>152</v>
+      </c>
+      <c r="H12">
+        <v>1268</v>
+      </c>
+      <c r="I12">
+        <v>217</v>
+      </c>
+      <c r="J12">
+        <v>1485</v>
+      </c>
+      <c r="K12">
+        <v>402.43900000000002</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2953</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>11.3725</v>
+      </c>
+      <c r="E13">
+        <v>10.642200000000001</v>
+      </c>
+      <c r="F13">
+        <v>510</v>
+      </c>
+      <c r="G13">
+        <v>58</v>
+      </c>
+      <c r="H13">
+        <v>487</v>
+      </c>
+      <c r="I13">
+        <v>452</v>
+      </c>
+      <c r="J13">
+        <v>939</v>
+      </c>
+      <c r="K13">
+        <v>184.11760000000001</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3005</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>1.9157</v>
+      </c>
+      <c r="E14">
+        <v>62.5</v>
+      </c>
+      <c r="F14">
+        <v>261</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>256</v>
+      </c>
+      <c r="J14">
+        <v>259</v>
+      </c>
+      <c r="K14">
+        <v>99.233699999999999</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2649</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>21.739100000000001</v>
+      </c>
+      <c r="E15">
+        <v>2.3641000000000001</v>
+      </c>
+      <c r="F15">
+        <v>46</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>413</v>
+      </c>
+      <c r="I15">
+        <v>36</v>
+      </c>
+      <c r="J15">
+        <v>449</v>
+      </c>
+      <c r="K15">
+        <v>976.08699999999999</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3251</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>109</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>109</v>
+      </c>
+      <c r="J16">
+        <v>117</v>
+      </c>
+      <c r="K16">
+        <v>107.3394</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2262</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>22.7273</v>
+      </c>
+      <c r="E17">
+        <v>2.2198000000000002</v>
+      </c>
+      <c r="F17">
+        <v>88</v>
+      </c>
+      <c r="G17">
+        <v>20</v>
+      </c>
+      <c r="H17">
+        <v>881</v>
+      </c>
+      <c r="I17">
+        <v>68</v>
+      </c>
+      <c r="J17">
+        <v>949</v>
+      </c>
+      <c r="K17">
+        <v>1078.4091000000001</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2208</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>84.145700000000005</v>
+      </c>
+      <c r="E18">
+        <v>92.303200000000004</v>
+      </c>
+      <c r="F18">
+        <v>1867</v>
+      </c>
+      <c r="G18">
+        <v>1571</v>
+      </c>
+      <c r="H18">
+        <v>131</v>
+      </c>
+      <c r="I18">
+        <v>296</v>
+      </c>
+      <c r="J18">
+        <v>427</v>
+      </c>
+      <c r="K18">
+        <v>22.870899999999999</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2154</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>34.782600000000002</v>
+      </c>
+      <c r="E19">
+        <v>1.5564</v>
+      </c>
+      <c r="F19">
+        <v>23</v>
+      </c>
+      <c r="G19">
+        <v>8</v>
+      </c>
+      <c r="H19">
+        <v>506</v>
+      </c>
+      <c r="I19">
+        <v>15</v>
+      </c>
+      <c r="J19">
+        <v>521</v>
+      </c>
+      <c r="K19">
+        <v>2265.2174</v>
+      </c>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2048</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>3.7037</v>
+      </c>
+      <c r="E20">
+        <v>0.11751</v>
+      </c>
+      <c r="F20">
+        <v>27</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>850</v>
+      </c>
+      <c r="I20">
+        <v>26</v>
+      </c>
+      <c r="J20">
+        <v>876</v>
+      </c>
+      <c r="K20">
+        <v>3244.4443999999999</v>
+      </c>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2427</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>46.875</v>
+      </c>
+      <c r="E21">
+        <v>3.5971000000000002</v>
+      </c>
+      <c r="F21">
+        <v>64</v>
+      </c>
+      <c r="G21">
+        <v>30</v>
+      </c>
+      <c r="H21">
+        <v>804</v>
+      </c>
+      <c r="I21">
+        <v>34</v>
+      </c>
+      <c r="J21">
+        <v>838</v>
+      </c>
+      <c r="K21">
+        <v>1309.375</v>
+      </c>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2483</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>42.204300000000003</v>
+      </c>
+      <c r="E22">
+        <v>42.547400000000003</v>
+      </c>
+      <c r="F22">
+        <v>372</v>
+      </c>
+      <c r="G22">
+        <v>157</v>
+      </c>
+      <c r="H22">
+        <v>212</v>
+      </c>
+      <c r="I22">
+        <v>215</v>
+      </c>
+      <c r="J22">
+        <v>427</v>
+      </c>
+      <c r="K22">
+        <v>114.78489999999999</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2605</v>
+      </c>
+      <c r="C23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>15.1869</v>
+      </c>
+      <c r="E23">
+        <v>32.6633</v>
+      </c>
+      <c r="F23">
+        <v>428</v>
+      </c>
+      <c r="G23">
+        <v>65</v>
+      </c>
+      <c r="H23">
+        <v>134</v>
+      </c>
+      <c r="I23">
+        <v>363</v>
+      </c>
+      <c r="J23">
+        <v>497</v>
+      </c>
+      <c r="K23">
+        <v>116.1215</v>
+      </c>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2053</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <v>58.883200000000002</v>
+      </c>
+      <c r="E24">
+        <v>42.413200000000003</v>
+      </c>
+      <c r="F24">
+        <v>394</v>
+      </c>
+      <c r="G24">
+        <v>232</v>
+      </c>
+      <c r="H24">
+        <v>315</v>
+      </c>
+      <c r="I24">
+        <v>162</v>
+      </c>
+      <c r="J24">
+        <v>477</v>
+      </c>
+      <c r="K24">
+        <v>121.066</v>
+      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2256</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25">
+        <v>49.070999999999998</v>
+      </c>
+      <c r="E25">
+        <v>63.150500000000001</v>
+      </c>
+      <c r="F25">
+        <v>915</v>
+      </c>
+      <c r="G25">
+        <v>449</v>
+      </c>
+      <c r="H25">
+        <v>262</v>
+      </c>
+      <c r="I25">
+        <v>466</v>
+      </c>
+      <c r="J25">
+        <v>728</v>
+      </c>
+      <c r="K25">
+        <v>79.562799999999996</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1571</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26">
+        <v>0.95238</v>
+      </c>
+      <c r="E26">
+        <v>19.047599999999999</v>
+      </c>
+      <c r="F26">
+        <v>420</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>17</v>
+      </c>
+      <c r="I26">
+        <v>416</v>
+      </c>
+      <c r="J26">
+        <v>433</v>
+      </c>
+      <c r="K26">
+        <v>103.09520000000001</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3079</v>
+      </c>
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27">
+        <v>52.631599999999999</v>
+      </c>
+      <c r="E27">
+        <v>14.005599999999999</v>
+      </c>
+      <c r="F27">
+        <v>190</v>
+      </c>
+      <c r="G27">
+        <v>100</v>
+      </c>
+      <c r="H27">
+        <v>614</v>
+      </c>
+      <c r="I27">
+        <v>90</v>
+      </c>
+      <c r="J27">
+        <v>704</v>
+      </c>
+      <c r="K27">
+        <v>370.52629999999999</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+    </row>
+    <row r="28" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1">
+        <v>2753</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>48</v>
+      </c>
+      <c r="J28">
+        <v>48</v>
+      </c>
+      <c r="K28">
+        <v>96</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+    </row>
+    <row r="29" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <f>SUM(B2:B28)</f>
+        <v>63690</v>
+      </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+    </row>
+    <row r="31" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+    </row>
+    <row r="32" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+    </row>
+    <row r="33" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+    </row>
+    <row r="34" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+    </row>
+    <row r="35" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+    </row>
+    <row r="36" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+    </row>
+    <row r="38" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+    </row>
+    <row r="39" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+    </row>
+    <row r="40" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+    </row>
+    <row r="41" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1"/>
+    </row>
+    <row r="42" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+    </row>
+    <row r="43" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+    </row>
+    <row r="44" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+    </row>
+    <row r="45" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+    </row>
+    <row r="46" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1"/>
+    </row>
+    <row r="47" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+    </row>
+    <row r="48" spans="13:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1"/>
+    </row>
+    <row r="49" spans="2:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+    </row>
+    <row r="50" spans="2:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="1"/>
+      <c r="S50" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8E8648-13CF-488F-AB80-4F7F6A86F737}">
+  <dimension ref="A1:K44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>69.115700000000004</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>2273</v>
+      </c>
+      <c r="F2">
+        <v>1571</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>702</v>
+      </c>
+      <c r="I2">
+        <v>702</v>
+      </c>
+      <c r="J2">
+        <v>30.8843</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>96.081599999999995</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>1863</v>
+      </c>
+      <c r="F3">
+        <v>1790</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>73</v>
+      </c>
+      <c r="I3">
+        <v>73</v>
+      </c>
+      <c r="J3">
+        <v>3.9184000000000001</v>
+      </c>
+      <c r="K3" s="1">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>64.7059</v>
+      </c>
+      <c r="D4">
+        <v>46.808500000000002</v>
+      </c>
+      <c r="E4">
+        <v>102</v>
+      </c>
+      <c r="F4">
+        <v>66</v>
+      </c>
+      <c r="G4">
+        <v>75</v>
+      </c>
+      <c r="H4">
+        <v>36</v>
+      </c>
+      <c r="I4">
+        <v>111</v>
+      </c>
+      <c r="J4">
+        <v>108.8235</v>
+      </c>
+      <c r="K4" s="1">
+        <v>2187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>73.512500000000003</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>2084</v>
+      </c>
+      <c r="F5">
+        <v>1532</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>552</v>
+      </c>
+      <c r="I5">
+        <v>552</v>
+      </c>
+      <c r="J5">
+        <v>26.487500000000001</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>17.993099999999998</v>
+      </c>
+      <c r="D6">
+        <v>36.1111</v>
+      </c>
+      <c r="E6">
+        <v>289</v>
+      </c>
+      <c r="F6">
+        <v>52</v>
+      </c>
+      <c r="G6">
+        <v>92</v>
+      </c>
+      <c r="H6">
+        <v>237</v>
+      </c>
+      <c r="I6">
+        <v>329</v>
+      </c>
+      <c r="J6">
+        <v>113.8408</v>
+      </c>
+      <c r="K6" s="1">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>11.858499999999999</v>
+      </c>
+      <c r="D7">
+        <v>99.673199999999994</v>
+      </c>
+      <c r="E7">
+        <v>2572</v>
+      </c>
+      <c r="F7">
+        <v>305</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2267</v>
+      </c>
+      <c r="I7">
+        <v>2268</v>
+      </c>
+      <c r="J7">
+        <v>88.180400000000006</v>
+      </c>
+      <c r="K7" s="1">
+        <v>2572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <v>49.966299999999997</v>
+      </c>
+      <c r="D8">
+        <v>99.865200000000002</v>
+      </c>
+      <c r="E8">
+        <v>1483</v>
+      </c>
+      <c r="F8">
+        <v>741</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>742</v>
+      </c>
+      <c r="I8">
+        <v>743</v>
+      </c>
+      <c r="J8">
+        <v>50.101100000000002</v>
+      </c>
+      <c r="K8" s="1">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>16.524699999999999</v>
+      </c>
+      <c r="D9">
+        <v>99.657499999999999</v>
+      </c>
+      <c r="E9">
+        <v>1761</v>
+      </c>
+      <c r="F9">
+        <v>291</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1470</v>
+      </c>
+      <c r="I9">
+        <v>1471</v>
+      </c>
+      <c r="J9">
+        <v>83.5321</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>3.4754999999999998</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>2532</v>
+      </c>
+      <c r="F10">
+        <v>88</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>2444</v>
+      </c>
+      <c r="I10">
+        <v>2444</v>
+      </c>
+      <c r="J10">
+        <v>96.524500000000003</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2532</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>1.1776</v>
+      </c>
+      <c r="D11">
+        <v>96.153800000000004</v>
+      </c>
+      <c r="E11">
+        <v>2123</v>
+      </c>
+      <c r="F11">
+        <v>25</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>2098</v>
+      </c>
+      <c r="I11">
+        <v>2099</v>
+      </c>
+      <c r="J11">
+        <v>98.869500000000002</v>
+      </c>
+      <c r="K11" s="1">
+        <v>2123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>25.758199999999999</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>2539</v>
+      </c>
+      <c r="F12">
+        <v>654</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>1885</v>
+      </c>
+      <c r="I12">
+        <v>1885</v>
+      </c>
+      <c r="J12">
+        <v>74.241799999999998</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2539</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>73.728300000000004</v>
+      </c>
+      <c r="D13">
+        <v>99.848600000000005</v>
+      </c>
+      <c r="E13">
+        <v>1789</v>
+      </c>
+      <c r="F13">
+        <v>1319</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>470</v>
+      </c>
+      <c r="I13">
+        <v>472</v>
+      </c>
+      <c r="J13">
+        <v>26.383500000000002</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>15.865399999999999</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14">
+        <v>1872</v>
+      </c>
+      <c r="F14">
+        <v>297</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1575</v>
+      </c>
+      <c r="I14">
+        <v>1575</v>
+      </c>
+      <c r="J14">
+        <v>84.134600000000006</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>84.894999999999996</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>1953</v>
+      </c>
+      <c r="F15">
+        <v>1658</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>295</v>
+      </c>
+      <c r="I15">
+        <v>295</v>
+      </c>
+      <c r="J15">
+        <v>15.105</v>
+      </c>
+      <c r="K15" s="1">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>56.799300000000002</v>
+      </c>
+      <c r="D16">
+        <v>100</v>
+      </c>
+      <c r="E16">
+        <v>2412</v>
+      </c>
+      <c r="F16">
+        <v>1370</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>1042</v>
+      </c>
+      <c r="I16">
+        <v>1042</v>
+      </c>
+      <c r="J16">
+        <v>43.200699999999998</v>
+      </c>
+      <c r="K16" s="1">
+        <v>2412</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>0.78176000000000001</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>1535</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1523</v>
+      </c>
+      <c r="I17">
+        <v>1523</v>
+      </c>
+      <c r="J17">
+        <v>99.218199999999996</v>
+      </c>
+      <c r="K17" s="1">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>35.136299999999999</v>
+      </c>
+      <c r="D18">
+        <v>100</v>
+      </c>
+      <c r="E18">
+        <v>2274</v>
+      </c>
+      <c r="F18">
+        <v>799</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1475</v>
+      </c>
+      <c r="I18">
+        <v>1475</v>
+      </c>
+      <c r="J18">
+        <v>64.863699999999994</v>
+      </c>
+      <c r="K18" s="1">
+        <v>2274</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19">
+        <v>63.7517</v>
+      </c>
+      <c r="D19">
+        <v>92.898799999999994</v>
+      </c>
+      <c r="E19">
+        <v>1498</v>
+      </c>
+      <c r="F19">
+        <v>955</v>
+      </c>
+      <c r="G19">
+        <v>73</v>
+      </c>
+      <c r="H19">
+        <v>543</v>
+      </c>
+      <c r="I19">
+        <v>616</v>
+      </c>
+      <c r="J19">
+        <v>41.121499999999997</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>21.846499999999999</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>1863</v>
+      </c>
+      <c r="F20">
+        <v>407</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1456</v>
+      </c>
+      <c r="I20">
+        <v>1456</v>
+      </c>
+      <c r="J20">
+        <v>78.153499999999994</v>
+      </c>
+      <c r="K20" s="1">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21">
+        <v>99.272999999999996</v>
+      </c>
+      <c r="D21">
+        <v>100</v>
+      </c>
+      <c r="E21">
+        <v>2476</v>
+      </c>
+      <c r="F21">
+        <v>2458</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>18</v>
+      </c>
+      <c r="I21">
+        <v>18</v>
+      </c>
+      <c r="J21">
+        <v>0.72697999999999996</v>
+      </c>
+      <c r="K21" s="1">
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <v>6.2582000000000004</v>
+      </c>
+      <c r="D22">
+        <v>100</v>
+      </c>
+      <c r="E22">
+        <v>1518</v>
+      </c>
+      <c r="F22">
+        <v>95</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1423</v>
+      </c>
+      <c r="I22">
+        <v>1423</v>
+      </c>
+      <c r="J22">
+        <v>93.741799999999998</v>
+      </c>
+      <c r="K22" s="1">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>11.929600000000001</v>
+      </c>
+      <c r="D23">
+        <v>94.329899999999995</v>
+      </c>
+      <c r="E23">
+        <v>1534</v>
+      </c>
+      <c r="F23">
+        <v>183</v>
+      </c>
+      <c r="G23">
+        <v>11</v>
+      </c>
+      <c r="H23">
+        <v>1351</v>
+      </c>
+      <c r="I23">
+        <v>1362</v>
+      </c>
+      <c r="J23">
+        <v>88.787499999999994</v>
+      </c>
+      <c r="K23" s="1">
+        <v>1619</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>27.4678</v>
+      </c>
+      <c r="D24">
+        <v>94.117599999999996</v>
+      </c>
+      <c r="E24">
+        <v>1398</v>
+      </c>
+      <c r="F24">
+        <v>384</v>
+      </c>
+      <c r="G24">
+        <v>24</v>
+      </c>
+      <c r="H24">
+        <v>1014</v>
+      </c>
+      <c r="I24">
+        <v>1038</v>
+      </c>
+      <c r="J24">
+        <v>74.248900000000006</v>
+      </c>
+      <c r="K24" s="1">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25">
+        <v>4.0639000000000003</v>
+      </c>
+      <c r="D25">
+        <v>15.6425</v>
+      </c>
+      <c r="E25">
+        <v>689</v>
+      </c>
+      <c r="F25">
+        <v>28</v>
+      </c>
+      <c r="G25">
+        <v>151</v>
+      </c>
+      <c r="H25">
+        <v>661</v>
+      </c>
+      <c r="I25">
+        <v>812</v>
+      </c>
+      <c r="J25">
+        <v>117.852</v>
+      </c>
+      <c r="K25" s="1">
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26">
+        <v>11.8132</v>
+      </c>
+      <c r="D26">
+        <v>65.816299999999998</v>
+      </c>
+      <c r="E26">
+        <v>1092</v>
+      </c>
+      <c r="F26">
+        <v>129</v>
+      </c>
+      <c r="G26">
+        <v>67</v>
+      </c>
+      <c r="H26">
+        <v>963</v>
+      </c>
+      <c r="I26">
+        <v>1030</v>
+      </c>
+      <c r="J26">
+        <v>94.322299999999998</v>
+      </c>
+      <c r="K26" s="1">
+        <v>2136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27">
+        <v>95.972399999999993</v>
+      </c>
+      <c r="D27">
+        <v>100</v>
+      </c>
+      <c r="E27">
+        <v>2607</v>
+      </c>
+      <c r="F27">
+        <v>2502</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>105</v>
+      </c>
+      <c r="I27">
+        <v>105</v>
+      </c>
+      <c r="J27">
+        <v>4.0275999999999996</v>
+      </c>
+      <c r="K27" s="1">
+        <v>2656</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28">
+        <v>0.3367</v>
+      </c>
+      <c r="D28">
+        <v>71.428600000000003</v>
+      </c>
+      <c r="E28">
+        <v>1485</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1480</v>
+      </c>
+      <c r="I28">
+        <v>1482</v>
+      </c>
+      <c r="J28">
+        <v>99.798000000000002</v>
+      </c>
+      <c r="K28" s="1">
+        <v>2332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29">
+        <v>10.438000000000001</v>
+      </c>
+      <c r="D29">
+        <v>65.051000000000002</v>
+      </c>
+      <c r="E29">
+        <v>2443</v>
+      </c>
+      <c r="F29">
+        <v>255</v>
+      </c>
+      <c r="G29">
+        <v>137</v>
+      </c>
+      <c r="H29">
+        <v>2188</v>
+      </c>
+      <c r="I29">
+        <v>2325</v>
+      </c>
+      <c r="J29">
+        <v>95.169899999999998</v>
+      </c>
+      <c r="K29" s="1">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <v>50.182200000000002</v>
+      </c>
+      <c r="D30">
+        <v>100</v>
+      </c>
+      <c r="E30">
+        <v>2744</v>
+      </c>
+      <c r="F30">
+        <v>1377</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1367</v>
+      </c>
+      <c r="I30">
+        <v>1367</v>
+      </c>
+      <c r="J30">
+        <v>49.817799999999998</v>
+      </c>
+      <c r="K30" s="1">
+        <v>3005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31">
+        <v>87.263499999999993</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+      <c r="E31">
+        <v>2748</v>
+      </c>
+      <c r="F31">
+        <v>2398</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>350</v>
+      </c>
+      <c r="I31">
+        <v>350</v>
+      </c>
+      <c r="J31">
+        <v>12.736499999999999</v>
+      </c>
+      <c r="K31" s="1">
+        <v>2748</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32">
+        <v>0.41466999999999998</v>
+      </c>
+      <c r="D32">
+        <v>100</v>
+      </c>
+      <c r="E32">
+        <v>3135</v>
+      </c>
+      <c r="F32">
+        <v>13</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>3122</v>
+      </c>
+      <c r="I32">
+        <v>3122</v>
+      </c>
+      <c r="J32">
+        <v>99.585300000000004</v>
+      </c>
+      <c r="K32" s="1">
+        <v>3251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>18.542400000000001</v>
+      </c>
+      <c r="D33">
+        <v>98.288499999999999</v>
+      </c>
+      <c r="E33">
+        <v>2168</v>
+      </c>
+      <c r="F33">
+        <v>402</v>
+      </c>
+      <c r="G33">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <v>1766</v>
+      </c>
+      <c r="I33">
+        <v>1773</v>
+      </c>
+      <c r="J33">
+        <v>81.7804</v>
+      </c>
+      <c r="K33" s="1">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34">
+        <v>0.47661999999999999</v>
+      </c>
+      <c r="D34">
+        <v>100</v>
+      </c>
+      <c r="E34">
+        <v>3357</v>
+      </c>
+      <c r="F34">
+        <v>16</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>3341</v>
+      </c>
+      <c r="I34">
+        <v>3341</v>
+      </c>
+      <c r="J34">
+        <v>99.523399999999995</v>
+      </c>
+      <c r="K34" s="1">
+        <v>3363</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35">
+        <v>6.0789999999999997</v>
+      </c>
+      <c r="D35">
+        <v>3.5148999999999999</v>
+      </c>
+      <c r="E35">
+        <v>329</v>
+      </c>
+      <c r="F35">
+        <v>20</v>
+      </c>
+      <c r="G35">
+        <v>549</v>
+      </c>
+      <c r="H35">
+        <v>309</v>
+      </c>
+      <c r="I35">
+        <v>858</v>
+      </c>
+      <c r="J35">
+        <v>260.7903</v>
+      </c>
+      <c r="K35" s="1">
+        <v>2154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>33.3003</v>
+      </c>
+      <c r="D36">
+        <v>99.851600000000005</v>
+      </c>
+      <c r="E36">
+        <v>2021</v>
+      </c>
+      <c r="F36">
+        <v>673</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1348</v>
+      </c>
+      <c r="I36">
+        <v>1349</v>
+      </c>
+      <c r="J36">
+        <v>66.749099999999999</v>
+      </c>
+      <c r="K36" s="1">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>68.924599999999998</v>
+      </c>
+      <c r="D37">
+        <v>91.666700000000006</v>
+      </c>
+      <c r="E37">
+        <v>1181</v>
+      </c>
+      <c r="F37">
+        <v>814</v>
+      </c>
+      <c r="G37">
+        <v>74</v>
+      </c>
+      <c r="H37">
+        <v>367</v>
+      </c>
+      <c r="I37">
+        <v>441</v>
+      </c>
+      <c r="J37">
+        <v>37.341200000000001</v>
+      </c>
+      <c r="K37" s="1">
+        <v>2483</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38">
+        <v>43.236499999999999</v>
+      </c>
+      <c r="D38">
+        <v>96.857500000000002</v>
+      </c>
+      <c r="E38">
+        <v>1996</v>
+      </c>
+      <c r="F38">
+        <v>863</v>
+      </c>
+      <c r="G38">
+        <v>28</v>
+      </c>
+      <c r="H38">
+        <v>1133</v>
+      </c>
+      <c r="I38">
+        <v>1161</v>
+      </c>
+      <c r="J38">
+        <v>58.1663</v>
+      </c>
+      <c r="K38" s="1">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39">
+        <v>10.428000000000001</v>
+      </c>
+      <c r="D39">
+        <v>98.857100000000003</v>
+      </c>
+      <c r="E39">
+        <v>1659</v>
+      </c>
+      <c r="F39">
+        <v>173</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>1486</v>
+      </c>
+      <c r="I39">
+        <v>1488</v>
+      </c>
+      <c r="J39">
+        <v>89.692599999999999</v>
+      </c>
+      <c r="K39" s="1">
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>61.148400000000002</v>
+      </c>
+      <c r="D40">
+        <v>93.714299999999994</v>
+      </c>
+      <c r="E40">
+        <v>1341</v>
+      </c>
+      <c r="F40">
+        <v>820</v>
+      </c>
+      <c r="G40">
+        <v>55</v>
+      </c>
+      <c r="H40">
+        <v>521</v>
+      </c>
+      <c r="I40">
+        <v>576</v>
+      </c>
+      <c r="J40">
+        <v>42.953000000000003</v>
+      </c>
+      <c r="K40" s="1">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41">
+        <v>90.790599999999998</v>
+      </c>
+      <c r="D41">
+        <v>100</v>
+      </c>
+      <c r="E41">
+        <v>1151</v>
+      </c>
+      <c r="F41">
+        <v>1045</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>106</v>
+      </c>
+      <c r="I41">
+        <v>106</v>
+      </c>
+      <c r="J41">
+        <v>9.2094000000000005</v>
+      </c>
+      <c r="K41" s="1">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42">
+        <v>5.8864999999999998</v>
+      </c>
+      <c r="D42">
+        <v>100</v>
+      </c>
+      <c r="E42">
+        <v>2871</v>
+      </c>
+      <c r="F42">
+        <v>169</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>2702</v>
+      </c>
+      <c r="I42">
+        <v>2702</v>
+      </c>
+      <c r="J42">
+        <v>94.113500000000002</v>
+      </c>
+      <c r="K42" s="1">
+        <v>3079</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43">
+        <v>95.708500000000001</v>
+      </c>
+      <c r="D43">
+        <v>99.884200000000007</v>
+      </c>
+      <c r="E43">
+        <v>2703</v>
+      </c>
+      <c r="F43">
+        <v>2587</v>
+      </c>
+      <c r="G43">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>116</v>
+      </c>
+      <c r="I43">
+        <v>119</v>
+      </c>
+      <c r="J43">
+        <v>4.4024999999999999</v>
+      </c>
+      <c r="K43" s="1">
+        <v>2753</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K44">
+        <f>SUM(K2:K43)</f>
+        <v>95765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>